<commit_message>
Worked on OpenFileScript.cs improved readability and efficiency
</commit_message>
<xml_diff>
--- a/Christian Stiehl/Timesheet.xlsx
+++ b/Christian Stiehl/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Set up GitHub directory, v0.1 READ ME and Timesheet. Started working on comments/code efficiency.</t>
+  </si>
+  <si>
+    <t>Worked on comments and code efficiency.</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +499,12 @@
       <c r="A3" s="1">
         <v>42893</v>
       </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -670,7 +679,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>SUM(B2:B36)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved README and FileOpener
</commit_message>
<xml_diff>
--- a/Christian Stiehl/Timesheet.xlsx
+++ b/Christian Stiehl/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Worked on comments and code efficiency.</t>
+  </si>
+  <si>
+    <t>Improved FileOpener readability and efficiency.</t>
   </si>
 </sst>
 </file>
@@ -463,7 +466,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +513,12 @@
       <c r="A4" s="1">
         <v>42923</v>
       </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -679,7 +688,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>SUM(B2:B36)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished writing summaries, added documentation generated with Doxygen.
</commit_message>
<xml_diff>
--- a/Christian Stiehl/Timesheet.xlsx
+++ b/Christian Stiehl/Timesheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Improved FileOpener readability and efficiency.</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>Finished comments &amp; summaries, added Doxygen code documentation to Git repository. Emailed Riemer about the direction of the project.</t>
   </si>
 </sst>
 </file>
@@ -466,14 +472,14 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="92" customWidth="1"/>
+    <col min="3" max="3" width="128.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,16 +530,34 @@
       <c r="A5" s="1">
         <v>42954</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42985</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43015</v>
       </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -688,7 +712,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>SUM(B2:B36)</f>
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tab switching now disables editing of the diagrams and more.
</commit_message>
<xml_diff>
--- a/Christian Stiehl/Timesheet.xlsx
+++ b/Christian Stiehl/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>Finished comments &amp; summaries, added Doxygen code documentation to Git repository. Emailed Riemer about the direction of the project.</t>
+  </si>
+  <si>
+    <t>Waiting for info from Riemer &amp; Anders</t>
+  </si>
+  <si>
+    <t>Meeting with Riemer &amp; Anders, License, Started working on the Interactive Tree View</t>
+  </si>
+  <si>
+    <t>Fixed hour proposition &amp; Emailed Riemer and Anders about meeting.</t>
+  </si>
+  <si>
+    <t>Worked on READ ME and Instructions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on tab selection and disabling editing when not in the editor tab. </t>
   </si>
 </sst>
 </file>
@@ -471,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,36 +578,78 @@
       <c r="A8" s="1">
         <v>43046</v>
       </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43076</v>
       </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -712,7 +769,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>SUM(B2:B36)</f>
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scrollable tree view & branch prefab
</commit_message>
<xml_diff>
--- a/Christian Stiehl/Timesheet.xlsx
+++ b/Christian Stiehl/Timesheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t xml:space="preserve">Worked on tab selection and disabling editing when not in the editor tab. </t>
+  </si>
+  <si>
+    <t>Fixed some bugs with editing disabling and tab selection</t>
+  </si>
+  <si>
+    <t>Added scrollable tree view &amp; branch item prefab</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,11 +661,23 @@
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -769,7 +787,7 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>SUM(B2:B36)</f>
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>